<commit_message>
added results and discussion for charging configurations
</commit_message>
<xml_diff>
--- a/papers/main_ees_outputs.xlsx
+++ b/papers/main_ees_outputs.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Desktop\Research\Paper\Data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Desktop\GitBash\neup-ies\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9A467B7-E089-4598-90FB-0725C523BCC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F69C3A-04F1-434E-9BB8-E0EF3D9A5A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{1724B149-890B-4624-B0D1-6DDBBEF1AB22}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{1724B149-890B-4624-B0D1-6DDBBEF1AB22}"/>
   </bookViews>
   <sheets>
     <sheet name="NonCharging" sheetId="10" r:id="rId1"/>
@@ -781,8 +781,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471CB529-8241-425E-A504-DD1217688B48}">
   <dimension ref="A1:AJ66"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:G3"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1041,7 +1041,7 @@
         <v>17</v>
       </c>
       <c r="E5" s="10">
-        <v>395.1</v>
+        <v>415.1</v>
       </c>
       <c r="F5" s="3" t="s">
         <v>17</v>
@@ -1083,7 +1083,7 @@
         <v>17</v>
       </c>
       <c r="S5">
-        <v>395.2</v>
+        <v>415.2</v>
       </c>
       <c r="T5" t="s">
         <v>17</v>
@@ -1760,7 +1760,7 @@
       <c r="V14" t="s">
         <v>17</v>
       </c>
-      <c r="W14" s="2">
+      <c r="W14" s="3">
         <v>0.5484</v>
       </c>
       <c r="X14" s="4" t="s">
@@ -2065,13 +2065,13 @@
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B19" t="s">
         <v>17</v>
       </c>
       <c r="C19" t="s">
-        <v>50</v>
+        <v>33</v>
       </c>
       <c r="D19" t="s">
         <v>17</v>
@@ -2139,13 +2139,13 @@
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A20" t="s">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="B20" t="s">
         <v>17</v>
       </c>
       <c r="C20" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="D20" t="s">
         <v>17</v>
@@ -2157,7 +2157,7 @@
         <v>17</v>
       </c>
       <c r="G20" s="10">
-        <v>0.9627</v>
+        <v>0.81430000000000002</v>
       </c>
       <c r="H20" t="s">
         <v>17</v>
@@ -2213,13 +2213,13 @@
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="B21" t="s">
         <v>17</v>
       </c>
       <c r="C21" t="s">
-        <v>52</v>
+        <v>35</v>
       </c>
       <c r="D21" t="s">
         <v>17</v>
@@ -2287,13 +2287,13 @@
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
-        <v>49</v>
+        <v>14</v>
       </c>
       <c r="B22" t="s">
         <v>17</v>
       </c>
       <c r="C22" t="s">
-        <v>53</v>
+        <v>36</v>
       </c>
       <c r="D22" t="s">
         <v>17</v>
@@ -2705,7 +2705,7 @@
         <v>17</v>
       </c>
       <c r="Q27" s="3">
-        <v>75.19</v>
+        <v>35.049999999999997</v>
       </c>
       <c r="R27" s="3" t="s">
         <v>17</v>
@@ -5440,7 +5440,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4DBDD3-036C-412E-B0AD-E5367CC713BE}">
   <dimension ref="A1:X79"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="A4" sqref="A4:P28"/>
     </sheetView>
   </sheetViews>
@@ -5837,7 +5837,7 @@
         <v>17</v>
       </c>
       <c r="I9" s="3">
-        <v>119</v>
+        <v>118.9</v>
       </c>
       <c r="J9" t="s">
         <v>17</v>
@@ -6175,7 +6175,7 @@
         <v>17</v>
       </c>
       <c r="E16" s="10">
-        <v>0.69899999999999995</v>
+        <v>6.99</v>
       </c>
       <c r="F16" t="s">
         <v>17</v>
@@ -6575,7 +6575,7 @@
         <v>17</v>
       </c>
       <c r="E24" s="10">
-        <v>0.90400000000000003</v>
+        <v>9.0399999999999991</v>
       </c>
       <c r="F24" t="s">
         <v>17</v>

</xml_diff>

<commit_message>
added TES charging techniques
</commit_message>
<xml_diff>
--- a/papers/main_ees_outputs.xlsx
+++ b/papers/main_ees_outputs.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\brian\Desktop\GitBash\neup-ies\papers\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E0F69C3A-04F1-434E-9BB8-E0EF3D9A5A00}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4CDBA14-1EBF-47C7-9D66-407D60234915}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" xr2:uid="{1724B149-890B-4624-B0D1-6DDBBEF1AB22}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="20715" windowHeight="13276" activeTab="1" xr2:uid="{1724B149-890B-4624-B0D1-6DDBBEF1AB22}"/>
   </bookViews>
   <sheets>
     <sheet name="NonCharging" sheetId="10" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4690" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4714" uniqueCount="131">
   <si>
     <t>Cold TES Temperature (K)</t>
   </si>
@@ -390,6 +390,51 @@
   </si>
   <si>
     <t>$T_{4,1C}$</t>
+  </si>
+  <si>
+    <t>Total  sCO$_2$ Mass Flow (kg/s)</t>
+  </si>
+  <si>
+    <t>Solar Mass Flow (kg/s)</t>
+  </si>
+  <si>
+    <t>$\dot{m}_{S3}$</t>
+  </si>
+  <si>
+    <t>$\dot{m}_{3}$</t>
+  </si>
+  <si>
+    <t>C2S UA Value (MW/$^{\circ}$C)</t>
+  </si>
+  <si>
+    <t>C2S Capacitance Ratio (-)</t>
+  </si>
+  <si>
+    <t>C2S Heat Transfer Rate (MW)</t>
+  </si>
+  <si>
+    <t>C2S Effectiveness (-)</t>
+  </si>
+  <si>
+    <t>C2S Approach Temperature ($^{\circ}$C)</t>
+  </si>
+  <si>
+    <t>$UA_{C2S}$</t>
+  </si>
+  <si>
+    <t>$CR_{C2S}$</t>
+  </si>
+  <si>
+    <t>$\dot{Q}_{C2S}$</t>
+  </si>
+  <si>
+    <t>$\varepsilon_{C2S}$</t>
+  </si>
+  <si>
+    <t>$\delta_{C2S}$</t>
+  </si>
+  <si>
+    <t>C2S Mass Flow Fraction (-)</t>
   </si>
 </sst>
 </file>
@@ -779,10 +824,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{471CB529-8241-425E-A504-DD1217688B48}">
-  <dimension ref="A1:AJ66"/>
+  <dimension ref="A1:AV66"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -813,7 +858,7 @@
     <col min="36" max="36" width="2.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -825,7 +870,7 @@
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
     </row>
-    <row r="2" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A2" s="1" t="s">
         <v>108</v>
       </c>
@@ -881,7 +926,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="3" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A3" s="1" t="s">
         <v>109</v>
       </c>
@@ -953,81 +998,95 @@
         <v>37</v>
       </c>
     </row>
-    <row r="4" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
-        <v>95</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>17</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>18</v>
+      <c r="C4" t="s">
+        <v>20</v>
       </c>
       <c r="D4" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="9" t="s">
-        <v>111</v>
-      </c>
-      <c r="F4" t="s">
-        <v>17</v>
-      </c>
-      <c r="G4" s="9" t="s">
-        <v>111</v>
+      <c r="E4" s="10">
+        <v>47.08</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="G4" s="10">
+        <v>45.28</v>
       </c>
       <c r="H4" t="s">
         <v>17</v>
       </c>
       <c r="I4" s="3">
-        <v>390</v>
+        <v>45.58</v>
       </c>
       <c r="J4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K4" s="3">
-        <v>440</v>
+        <v>45.93</v>
       </c>
       <c r="L4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="M4" s="3">
-        <v>390</v>
+        <v>44.9</v>
       </c>
       <c r="N4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="O4" s="3">
-        <v>410</v>
+        <v>44.22</v>
       </c>
       <c r="P4" s="3" t="s">
         <v>17</v>
       </c>
       <c r="Q4" s="3">
-        <v>440</v>
+        <v>44.22</v>
       </c>
       <c r="R4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S4">
-        <v>390</v>
+      <c r="S4" s="5">
+        <v>46.1</v>
       </c>
       <c r="T4" t="s">
         <v>17</v>
       </c>
       <c r="U4">
-        <v>390</v>
+        <v>44.34</v>
       </c>
       <c r="V4" t="s">
         <v>17</v>
       </c>
       <c r="W4">
-        <v>440</v>
+        <v>44.35</v>
       </c>
       <c r="X4" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="5" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="AA4" s="7"/>
+      <c r="AC4" s="9"/>
+      <c r="AE4" s="9"/>
+      <c r="AG4" s="3"/>
+      <c r="AH4" s="3"/>
+      <c r="AI4" s="3"/>
+      <c r="AJ4" s="3"/>
+      <c r="AK4" s="3"/>
+      <c r="AL4" s="3"/>
+      <c r="AM4" s="3"/>
+      <c r="AN4" s="3"/>
+      <c r="AO4" s="3"/>
+      <c r="AP4" s="3"/>
+      <c r="AV4" s="4"/>
+    </row>
+    <row r="5" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>96</v>
       </c>
@@ -1100,82 +1159,111 @@
       <c r="X5" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="6" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="AC5" s="10"/>
+      <c r="AD5" s="3"/>
+      <c r="AE5" s="10"/>
+      <c r="AG5" s="10"/>
+      <c r="AH5" s="3"/>
+      <c r="AI5" s="10"/>
+      <c r="AJ5" s="3"/>
+      <c r="AK5" s="3"/>
+      <c r="AL5" s="3"/>
+      <c r="AM5" s="3"/>
+      <c r="AN5" s="3"/>
+      <c r="AO5" s="3"/>
+      <c r="AP5" s="3"/>
+      <c r="AV5" s="4"/>
+    </row>
+    <row r="6" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A6" t="s">
-        <v>2</v>
+        <v>95</v>
       </c>
       <c r="B6" t="s">
         <v>17</v>
       </c>
-      <c r="C6" t="s">
-        <v>20</v>
+      <c r="C6" s="7" t="s">
+        <v>18</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
       </c>
-      <c r="E6" s="10">
-        <v>47.08</v>
-      </c>
-      <c r="F6" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="G6" s="10">
-        <v>45.28</v>
+      <c r="E6" s="9" t="s">
+        <v>111</v>
+      </c>
+      <c r="F6" t="s">
+        <v>17</v>
+      </c>
+      <c r="G6" s="9" t="s">
+        <v>111</v>
       </c>
       <c r="H6" t="s">
         <v>17</v>
       </c>
       <c r="I6" s="3">
-        <v>45.58</v>
+        <v>390</v>
       </c>
       <c r="J6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="K6" s="3">
-        <v>45.93</v>
+        <v>440</v>
       </c>
       <c r="L6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="M6" s="3">
-        <v>44.9</v>
+        <v>390</v>
       </c>
       <c r="N6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="O6" s="3">
-        <v>44.22</v>
+        <v>410</v>
       </c>
       <c r="P6" s="3" t="s">
         <v>17</v>
       </c>
       <c r="Q6" s="3">
-        <v>44.22</v>
+        <v>440</v>
       </c>
       <c r="R6" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="S6" s="5">
-        <v>46.1</v>
+      <c r="S6">
+        <v>390</v>
       </c>
       <c r="T6" t="s">
         <v>17</v>
       </c>
       <c r="U6">
-        <v>44.34</v>
+        <v>390</v>
       </c>
       <c r="V6" t="s">
         <v>17</v>
       </c>
       <c r="W6">
-        <v>44.35</v>
+        <v>440</v>
       </c>
       <c r="X6" s="4" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="AC6" s="10"/>
+      <c r="AD6" s="3"/>
+      <c r="AE6" s="10"/>
+      <c r="AG6" s="3"/>
+      <c r="AH6" s="3"/>
+      <c r="AI6" s="3"/>
+      <c r="AJ6" s="3"/>
+      <c r="AK6" s="3"/>
+      <c r="AL6" s="3"/>
+      <c r="AM6" s="3"/>
+      <c r="AN6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AP6" s="3"/>
+      <c r="AQ6" s="5"/>
+      <c r="AV6" s="4"/>
+    </row>
+    <row r="7" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A7" t="s">
         <v>83</v>
       </c>
@@ -1249,7 +1337,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="8" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>85</v>
       </c>
@@ -1323,7 +1411,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="9" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -1397,7 +1485,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="10" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A10" t="s">
         <v>86</v>
       </c>
@@ -1471,7 +1559,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A11" t="s">
         <v>91</v>
       </c>
@@ -1545,7 +1633,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A12" t="s">
         <v>92</v>
       </c>
@@ -1619,7 +1707,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="13" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -1693,7 +1781,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="14" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>75</v>
       </c>
@@ -1767,7 +1855,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="15" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>99</v>
       </c>
@@ -1841,7 +1929,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="16" spans="1:24" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:48" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>29</v>
       </c>
@@ -2948,6 +3036,94 @@
         <v>0.94930000000000003</v>
       </c>
       <c r="X30" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="31" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A31" t="s">
+        <v>116</v>
+      </c>
+      <c r="B31" t="s">
+        <v>17</v>
+      </c>
+      <c r="C31" t="s">
+        <v>119</v>
+      </c>
+      <c r="D31" t="s">
+        <v>17</v>
+      </c>
+      <c r="F31" t="s">
+        <v>17</v>
+      </c>
+      <c r="H31" t="s">
+        <v>17</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R31" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T31" t="s">
+        <v>17</v>
+      </c>
+      <c r="V31" t="s">
+        <v>17</v>
+      </c>
+      <c r="X31" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:24" x14ac:dyDescent="0.45">
+      <c r="A32" t="s">
+        <v>117</v>
+      </c>
+      <c r="B32" t="s">
+        <v>17</v>
+      </c>
+      <c r="C32" t="s">
+        <v>118</v>
+      </c>
+      <c r="D32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F32" t="s">
+        <v>17</v>
+      </c>
+      <c r="H32" t="s">
+        <v>17</v>
+      </c>
+      <c r="J32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="L32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="N32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="P32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="R32" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="T32" t="s">
+        <v>17</v>
+      </c>
+      <c r="V32" t="s">
+        <v>17</v>
+      </c>
+      <c r="X32" s="4" t="s">
         <v>37</v>
       </c>
     </row>
@@ -5423,16 +5599,18 @@
     <hyperlink ref="AJ63:AJ66" r:id="rId12" display="\\" xr:uid="{F7DE336F-89BE-42CF-8B3D-D6CD622021B5}"/>
     <hyperlink ref="AJ47" r:id="rId13" xr:uid="{67134FBD-6AEF-477E-A0A4-C7FBF9B12E4B}"/>
     <hyperlink ref="AJ50" r:id="rId14" xr:uid="{6D96B786-8080-4DA5-A0E3-F14070A5573F}"/>
-    <hyperlink ref="X4" r:id="rId15" xr:uid="{D6C4F046-42FE-4D31-BC8E-F3EB42579B57}"/>
-    <hyperlink ref="X5:X22" r:id="rId16" display="\\" xr:uid="{943771C5-864B-49CA-9B75-B0A8DA960961}"/>
-    <hyperlink ref="X23:X26" r:id="rId17" display="\\" xr:uid="{FDE99847-AB58-469D-80E0-0EC64B13DE41}"/>
-    <hyperlink ref="X27:X30" r:id="rId18" display="\\" xr:uid="{03D1AB31-E277-4895-8264-68B6A3CBEDC4}"/>
-    <hyperlink ref="X11" r:id="rId19" xr:uid="{42916071-32D6-443B-9C11-152B3E797217}"/>
-    <hyperlink ref="X14" r:id="rId20" xr:uid="{D4BC50DE-4B12-49B9-A638-0E43DD4FF2BE}"/>
-    <hyperlink ref="X2:X3" r:id="rId21" display="\\" xr:uid="{21DEF9B6-13AF-4F70-BB8B-3ECBB3A1F3A5}"/>
+    <hyperlink ref="X5:X22" r:id="rId15" display="\\" xr:uid="{943771C5-864B-49CA-9B75-B0A8DA960961}"/>
+    <hyperlink ref="X23:X26" r:id="rId16" display="\\" xr:uid="{FDE99847-AB58-469D-80E0-0EC64B13DE41}"/>
+    <hyperlink ref="X27:X30" r:id="rId17" display="\\" xr:uid="{03D1AB31-E277-4895-8264-68B6A3CBEDC4}"/>
+    <hyperlink ref="X11" r:id="rId18" xr:uid="{42916071-32D6-443B-9C11-152B3E797217}"/>
+    <hyperlink ref="X14" r:id="rId19" xr:uid="{D4BC50DE-4B12-49B9-A638-0E43DD4FF2BE}"/>
+    <hyperlink ref="X2:X3" r:id="rId20" display="\\" xr:uid="{21DEF9B6-13AF-4F70-BB8B-3ECBB3A1F3A5}"/>
+    <hyperlink ref="X4" r:id="rId21" xr:uid="{E4026EC1-39A9-4790-9542-7175AAA34077}"/>
+    <hyperlink ref="X6" r:id="rId22" xr:uid="{FC1482ED-A54E-4DBC-85B9-38580E8024BC}"/>
+    <hyperlink ref="X31:X32" r:id="rId23" display="\\" xr:uid="{8AA22F4D-F623-4630-975A-8AF9D18D7CB1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId22"/>
+  <pageSetup orientation="portrait" r:id="rId24"/>
 </worksheet>
 </file>
 
@@ -5440,8 +5618,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E4DBDD3-036C-412E-B0AD-E5367CC713BE}">
   <dimension ref="A1:X79"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A4" sqref="A4:P28"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -6063,7 +6241,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
-        <v>77</v>
+        <v>130</v>
       </c>
       <c r="B14" t="s">
         <v>17</v>
@@ -6563,13 +6741,13 @@
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
-        <v>97</v>
+        <v>120</v>
       </c>
       <c r="B24" t="s">
         <v>17</v>
       </c>
       <c r="C24" t="s">
-        <v>62</v>
+        <v>125</v>
       </c>
       <c r="D24" t="s">
         <v>17</v>
@@ -6613,13 +6791,13 @@
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
-        <v>59</v>
+        <v>121</v>
       </c>
       <c r="B25" t="s">
         <v>17</v>
       </c>
       <c r="C25" t="s">
-        <v>63</v>
+        <v>126</v>
       </c>
       <c r="D25" t="s">
         <v>17</v>
@@ -6663,13 +6841,13 @@
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
-        <v>90</v>
+        <v>122</v>
       </c>
       <c r="B26" t="s">
         <v>17</v>
       </c>
       <c r="C26" t="s">
-        <v>64</v>
+        <v>127</v>
       </c>
       <c r="D26" t="s">
         <v>17</v>
@@ -6713,13 +6891,13 @@
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A27" t="s">
-        <v>61</v>
+        <v>123</v>
       </c>
       <c r="B27" t="s">
         <v>17</v>
       </c>
       <c r="C27" t="s">
-        <v>65</v>
+        <v>128</v>
       </c>
       <c r="D27" t="s">
         <v>17</v>
@@ -6763,19 +6941,19 @@
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
-        <v>102</v>
+        <v>124</v>
       </c>
       <c r="B28" t="s">
         <v>17</v>
       </c>
       <c r="C28" t="s">
-        <v>79</v>
+        <v>129</v>
       </c>
       <c r="D28" t="s">
         <v>17</v>
       </c>
-      <c r="E28" s="9" t="s">
-        <v>111</v>
+      <c r="E28" s="9">
+        <v>10</v>
       </c>
       <c r="F28" t="s">
         <v>17</v>
@@ -6792,20 +6970,20 @@
       <c r="J28" t="s">
         <v>17</v>
       </c>
-      <c r="K28" s="9" t="s">
-        <v>111</v>
+      <c r="K28" s="9">
+        <v>10</v>
       </c>
       <c r="L28" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="M28" s="9" t="s">
-        <v>111</v>
+      <c r="M28" s="9">
+        <v>10</v>
       </c>
       <c r="N28" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="O28" s="9" t="s">
-        <v>111</v>
+      <c r="O28" s="9">
+        <v>10</v>
       </c>
       <c r="P28" s="4" t="s">
         <v>37</v>

</xml_diff>